<commit_message>
add USA fix 2
</commit_message>
<xml_diff>
--- a/Policy note/deficitcomptable.USA.xlsx
+++ b/Policy note/deficitcomptable.USA.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
-    <t>dc_real</t>
+    <t>BOGZ1FU315000005A</t>
   </si>
   <si>
     <t>period</t>
@@ -543,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>-104004000000</v>
+        <v>-104004</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>-88425000000</v>
+        <v>-88425</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -559,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>-86496000000</v>
+        <v>-86496</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -567,7 +567,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>-74643000000</v>
+        <v>-74643</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -575,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>-61047000000</v>
+        <v>-61047</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -583,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>-99531000000</v>
+        <v>-99531</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -591,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>-115265000000</v>
+        <v>-115265</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -599,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>-194628000000</v>
+        <v>-194628</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -607,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>-231009000000</v>
+        <v>-231009</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -615,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>-239200000000</v>
+        <v>-239200</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -623,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>-267154000000</v>
+        <v>-267154</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -631,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-292966000000</v>
+        <v>-292966</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -639,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-223009000000</v>
+        <v>-223009</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -647,7 +647,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>-242951000000</v>
+        <v>-242951</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -655,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>-246713000000</v>
+        <v>-246713</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -663,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>-259940000000</v>
+        <v>-259940</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -671,7 +671,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>-330976000000</v>
+        <v>-330976</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -679,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>-408235000000</v>
+        <v>-408235</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -687,7 +687,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>-337051000000</v>
+        <v>-337051</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -695,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>-261698000000</v>
+        <v>-261698</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -703,7 +703,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>-248905000000</v>
+        <v>-248905</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -711,7 +711,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>-186811000000</v>
+        <v>-186811</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -719,7 +719,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>-81988000000</v>
+        <v>-81988</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -727,7 +727,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>-17639000000</v>
+        <v>-17639</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -735,7 +735,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>72141000000</v>
+        <v>72141</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -743,7 +743,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>142759000000</v>
+        <v>142759</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -751,7 +751,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>-15773000000</v>
+        <v>-15773</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -759,7 +759,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>-315788000000</v>
+        <v>-315788</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -767,7 +767,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>-520795000000</v>
+        <v>-520795</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -775,7 +775,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>-476038000000</v>
+        <v>-476038</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -783,7 +783,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>-425109000000</v>
+        <v>-425109</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -791,7 +791,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>-312002000000</v>
+        <v>-312002</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -799,7 +799,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>-372342000000</v>
+        <v>-372342</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -807,7 +807,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>-768716000000</v>
+        <v>-768716</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -815,7 +815,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>-1330120000000</v>
+        <v>-1330120</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -823,7 +823,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>-1397199000000</v>
+        <v>-1397199</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -831,7 +831,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>-1327115000000</v>
+        <v>-1327115</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -839,7 +839,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>-1165319000000</v>
+        <v>-1165319</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -847,7 +847,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>-511794000000</v>
+        <v>-511794</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -855,7 +855,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>-742342000000</v>
+        <v>-742342</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -863,7 +863,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>-528890000000</v>
+        <v>-528890</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -871,7 +871,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>-687376000000</v>
+        <v>-687376</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -879,7 +879,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>-519859000000</v>
+        <v>-519859</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -887,7 +887,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>-969937000000</v>
+        <v>-969937</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -895,7 +895,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>-1113551000000</v>
+        <v>-1113551</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -903,7 +903,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>-3296254000000</v>
+        <v>-3296254</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -911,7 +911,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>-2688667000000</v>
+        <v>-2688667</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -919,7 +919,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>-1269138000000</v>
+        <v>-1269138</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -927,7 +927,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>-2342485000000</v>
+        <v>-2342485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>